<commit_message>
design improvements to UI
</commit_message>
<xml_diff>
--- a/data/project_db.xlsx
+++ b/data/project_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\cdss-dev-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C69A2-24D5-4BC5-83DE-C9DCBA8E3367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3916BC18-3FD4-42A9-9155-749B09D69C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm"/>
     <numFmt numFmtId="165" formatCode="[$-1010409]d/m/yyyy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,6 +187,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -238,6 +244,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,12 +258,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-1010409]d/m/yyyy\ h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
@@ -307,6 +310,12 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -321,18 +330,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}" name="Table1" displayName="Table1" ref="A1:H257" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}" name="Table1" displayName="Table1" ref="A1:H257" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H257" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H257">
     <sortCondition ref="A1:A257"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{EF889FAC-9E6F-4740-A706-7430617E85B5}" name="First name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{28F816C7-879A-40F5-B1CF-3F8CD0D44EA7}" name="Last name" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{2F676C46-3D00-4A27-A9F6-C2FA1A6DA6E0}" name="PatientId" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3BE22C6D-6D9C-471E-A0F7-427FE25E9550}" name="LOINC-NUM" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{55E39471-B051-4B6E-972D-C4E9F951DF55}" name="Value" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6E1661D5-D91B-472B-B184-95879FF2B22A}" name="Unit" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{EF889FAC-9E6F-4740-A706-7430617E85B5}" name="First name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{28F816C7-879A-40F5-B1CF-3F8CD0D44EA7}" name="Last name" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{2F676C46-3D00-4A27-A9F6-C2FA1A6DA6E0}" name="PatientId" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{3BE22C6D-6D9C-471E-A0F7-427FE25E9550}" name="LOINC-NUM" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{55E39471-B051-4B6E-972D-C4E9F951DF55}" name="Value" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6E1661D5-D91B-472B-B184-95879FF2B22A}" name="Unit" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{99C0158C-F3E2-4530-BE25-8BBB57894E98}" name="Valid start time" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{9189A167-024F-4E01-B352-B12A9FCCB680}" name="Transaction time" dataDxfId="0"/>
   </tableColumns>
@@ -629,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K271"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="175" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4674,10 +4683,10 @@
       <c r="K139" s="2"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C140" s="5">

</xml_diff>

<commit_message>
adding test to __main_
</commit_message>
<xml_diff>
--- a/data/project_db.xlsx
+++ b/data/project_db.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\cdss-dev-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE216C2F-5AED-4CE2-B32C-F2DC5843CED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85158E79-C8DF-4D4E-8A6A-B290123D07FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="2" r:id="rId1"/>
     <sheet name="Measurements" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Measurements!$A$1:$F$1158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Measurements!$A$1:$F$1224</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="86">
   <si>
     <t>Value</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Bronchospasm</t>
   </si>
   <si>
-    <t>Â°C</t>
-  </si>
-  <si>
     <t>Desquamation</t>
   </si>
   <si>
@@ -273,6 +270,18 @@
   </si>
   <si>
     <t>Sex</t>
+  </si>
+  <si>
+    <t>Sever-Bronchospasm</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -327,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -371,6 +380,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,8 +458,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}" name="Table1" displayName="Table1" ref="A1:F1158" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F1158" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}" name="Table1" displayName="Table1" ref="A1:F1224" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F1224" xr:uid="{368421E4-8352-48AB-B35B-E960839CEFF4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F1158">
     <sortCondition ref="A2:A1158"/>
     <sortCondition ref="E2:E1158"/>
@@ -755,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4F158B-403D-472C-9BD6-CE22F0137559}">
   <dimension ref="A1:D271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -778,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,10 +1044,18 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
+      <c r="A20" s="11">
+        <v>147258369</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21"/>
@@ -1357,15 +1375,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1158"/>
+  <dimension ref="A1:I1224"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1152" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A1158" sqref="A1158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="5" customWidth="1"/>
     <col min="4" max="4" width="16" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" style="5" bestFit="1" customWidth="1"/>
@@ -3081,7 +3101,7 @@
         <v>4438.5</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E75" s="6">
         <v>45704.655717592592</v>
@@ -3288,7 +3308,7 @@
         <v>5710.59</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E84" s="6">
         <v>45704.822384259256</v>
@@ -3495,7 +3515,7 @@
         <v>4468.5600000000004</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E93" s="6">
         <v>45704.989050925928</v>
@@ -3679,7 +3699,7 @@
         <v>3245.77</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E101" s="6">
         <v>45705.155717592592</v>
@@ -3745,7 +3765,7 @@
         <v>23924001</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>21</v>
@@ -3794,7 +3814,7 @@
         <v>8960.4599999999991</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E106" s="6">
         <v>45705.322384259256</v>
@@ -3929,7 +3949,7 @@
         <v>368009</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D112" s="14" t="s">
         <v>21</v>
@@ -3952,7 +3972,7 @@
         <v>23924001</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D113" s="14" t="s">
         <v>21</v>
@@ -4090,7 +4110,7 @@
         <v>368009</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D119" s="14" t="s">
         <v>21</v>
@@ -4251,7 +4271,7 @@
         <v>368009</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D126" s="14" t="s">
         <v>21</v>
@@ -4274,7 +4294,7 @@
         <v>23924001</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D127" s="14" t="s">
         <v>21</v>
@@ -4552,8 +4572,8 @@
       <c r="C139" s="9">
         <v>37.54</v>
       </c>
-      <c r="D139" s="14" t="s">
-        <v>75</v>
+      <c r="D139" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E139" s="6">
         <v>45505.655717592592</v>
@@ -4713,8 +4733,8 @@
       <c r="C146" s="9">
         <v>39.03</v>
       </c>
-      <c r="D146" s="14" t="s">
-        <v>75</v>
+      <c r="D146" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E146" s="6">
         <v>45505.822384259256</v>
@@ -4874,8 +4894,8 @@
       <c r="C153" s="9">
         <v>36.049999999999997</v>
       </c>
-      <c r="D153" s="14" t="s">
-        <v>75</v>
+      <c r="D153" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E153" s="6">
         <v>45505.989050925928</v>
@@ -5127,8 +5147,8 @@
       <c r="C164" s="8">
         <v>39.630000000000003</v>
       </c>
-      <c r="D164" s="9" t="s">
-        <v>75</v>
+      <c r="D164" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E164" s="6">
         <v>45607.655717592592</v>
@@ -5242,8 +5262,8 @@
       <c r="C169" s="8">
         <v>36.950000000000003</v>
       </c>
-      <c r="D169" s="9" t="s">
-        <v>75</v>
+      <c r="D169" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E169" s="6">
         <v>45607.905717592592</v>
@@ -5357,8 +5377,8 @@
       <c r="C174" s="8">
         <v>38.21</v>
       </c>
-      <c r="D174" s="9" t="s">
-        <v>75</v>
+      <c r="D174" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E174" s="6">
         <v>45608.155717592592</v>
@@ -5449,8 +5469,8 @@
       <c r="C178" s="8">
         <v>39.78</v>
       </c>
-      <c r="D178" s="9" t="s">
-        <v>75</v>
+      <c r="D178" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E178" s="6">
         <v>45608.405717592592</v>
@@ -5541,8 +5561,8 @@
       <c r="C182" s="8">
         <v>37.06</v>
       </c>
-      <c r="D182" s="9" t="s">
-        <v>75</v>
+      <c r="D182" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E182" s="6">
         <v>45608.655717592592</v>
@@ -5633,8 +5653,8 @@
       <c r="C186" s="8">
         <v>36.25</v>
       </c>
-      <c r="D186" s="9" t="s">
-        <v>75</v>
+      <c r="D186" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E186" s="6">
         <v>45608.905717592592</v>
@@ -6761,7 +6781,7 @@
         <v>4115.8100000000004</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E235" s="6">
         <v>45802.655717592592</v>
@@ -6827,7 +6847,7 @@
         <v>368009</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D238" s="14" t="s">
         <v>21</v>
@@ -6991,7 +7011,7 @@
         <v>13437.2</v>
       </c>
       <c r="D245" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E245" s="6">
         <v>45802.822384259256</v>
@@ -7057,7 +7077,7 @@
         <v>368009</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D248" s="14" t="s">
         <v>21</v>
@@ -7221,7 +7241,7 @@
         <v>13470.63</v>
       </c>
       <c r="D255" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E255" s="6">
         <v>45802.989050925928</v>
@@ -7287,7 +7307,7 @@
         <v>368009</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D258" s="14" t="s">
         <v>21</v>
@@ -7444,7 +7464,7 @@
         <v>9120.1200000000008</v>
       </c>
       <c r="D265" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E265" s="6">
         <v>45803.155717592592</v>
@@ -7532,7 +7552,7 @@
         <v>6287.36</v>
       </c>
       <c r="D269" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E269" s="6">
         <v>45803.322384259256</v>
@@ -8535,7 +8555,7 @@
         <v>368009</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D319" s="14" t="s">
         <v>21</v>
@@ -8578,7 +8598,7 @@
         <v>1339.24</v>
       </c>
       <c r="D321" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E321" s="6">
         <v>45601.655717592592</v>
@@ -8655,7 +8675,7 @@
         <v>368009</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D325" s="14" t="s">
         <v>21</v>
@@ -8698,7 +8718,7 @@
         <v>6047.08</v>
       </c>
       <c r="D327" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E327" s="6">
         <v>45601.822384259256</v>
@@ -8775,7 +8795,7 @@
         <v>368009</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D331" s="14" t="s">
         <v>21</v>
@@ -8818,7 +8838,7 @@
         <v>7852.04</v>
       </c>
       <c r="D333" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E333" s="6">
         <v>45601.989050925928</v>
@@ -8898,7 +8918,7 @@
         <v>2317.59</v>
       </c>
       <c r="D337" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E337" s="6">
         <v>45602.155717592592</v>
@@ -9115,7 +9135,7 @@
         <v>368009</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D348" s="14" t="s">
         <v>21</v>
@@ -9157,8 +9177,8 @@
       <c r="C350" s="9">
         <v>30.29</v>
       </c>
-      <c r="D350" s="14" t="s">
-        <v>75</v>
+      <c r="D350" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E350" s="6">
         <v>45576.655717592592</v>
@@ -9255,7 +9275,7 @@
         <v>368009</v>
       </c>
       <c r="C355" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D355" s="14" t="s">
         <v>21</v>
@@ -9297,8 +9317,8 @@
       <c r="C357" s="9">
         <v>37.03</v>
       </c>
-      <c r="D357" s="14" t="s">
-        <v>75</v>
+      <c r="D357" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E357" s="6">
         <v>45576.822384259256</v>
@@ -9395,7 +9415,7 @@
         <v>368009</v>
       </c>
       <c r="C362" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D362" s="14" t="s">
         <v>21</v>
@@ -9437,8 +9457,8 @@
       <c r="C364" s="9">
         <v>39.76</v>
       </c>
-      <c r="D364" s="14" t="s">
-        <v>75</v>
+      <c r="D364" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E364" s="6">
         <v>45576.989050925928</v>
@@ -9617,8 +9637,8 @@
       <c r="C373" s="8">
         <v>26.71</v>
       </c>
-      <c r="D373" s="9" t="s">
-        <v>75</v>
+      <c r="D373" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E373" s="6">
         <v>45784.655717592592</v>
@@ -9717,8 +9737,8 @@
       <c r="C378" s="8">
         <v>39.700000000000003</v>
       </c>
-      <c r="D378" s="9" t="s">
-        <v>75</v>
+      <c r="D378" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E378" s="6">
         <v>45784.905717592592</v>
@@ -9817,8 +9837,8 @@
       <c r="C383" s="8">
         <v>40.6</v>
       </c>
-      <c r="D383" s="9" t="s">
-        <v>75</v>
+      <c r="D383" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E383" s="6">
         <v>45785.155717592592</v>
@@ -9917,8 +9937,8 @@
       <c r="C388" s="8">
         <v>39.53</v>
       </c>
-      <c r="D388" s="9" t="s">
-        <v>75</v>
+      <c r="D388" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E388" s="6">
         <v>45785.405717592592</v>
@@ -9977,8 +9997,8 @@
       <c r="C391" s="8">
         <v>36.659999999999997</v>
       </c>
-      <c r="D391" s="9" t="s">
-        <v>75</v>
+      <c r="D391" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E391" s="6">
         <v>45785.655717592592</v>
@@ -10037,8 +10057,8 @@
       <c r="C394" s="8">
         <v>37.32</v>
       </c>
-      <c r="D394" s="9" t="s">
-        <v>75</v>
+      <c r="D394" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E394" s="6">
         <v>45785.905717592592</v>
@@ -10275,7 +10295,7 @@
         <v>368009</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D406" s="14" t="s">
         <v>21</v>
@@ -10435,7 +10455,7 @@
         <v>368009</v>
       </c>
       <c r="C414" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D414" s="14" t="s">
         <v>21</v>
@@ -10595,7 +10615,7 @@
         <v>368009</v>
       </c>
       <c r="C422" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D422" s="14" t="s">
         <v>21</v>
@@ -10695,7 +10715,7 @@
         <v>368009</v>
       </c>
       <c r="C427" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D427" s="14" t="s">
         <v>21</v>
@@ -10818,7 +10838,7 @@
         <v>0</v>
       </c>
       <c r="D433" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E433" s="6">
         <v>45680.655717592592</v>
@@ -10835,7 +10855,7 @@
         <v>368009</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D434" s="14" t="s">
         <v>21</v>
@@ -11018,7 +11038,7 @@
         <v>10662.1</v>
       </c>
       <c r="D443" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E443" s="6">
         <v>45680.822384259256</v>
@@ -11035,7 +11055,7 @@
         <v>368009</v>
       </c>
       <c r="C444" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D444" s="14" t="s">
         <v>21</v>
@@ -11218,7 +11238,7 @@
         <v>13860.13</v>
       </c>
       <c r="D453" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E453" s="6">
         <v>45680.989050925928</v>
@@ -11235,7 +11255,7 @@
         <v>368009</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D454" s="14" t="s">
         <v>21</v>
@@ -11255,7 +11275,7 @@
         <v>23924001</v>
       </c>
       <c r="C455" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D455" s="14" t="s">
         <v>21</v>
@@ -11418,7 +11438,7 @@
         <v>20394.28</v>
       </c>
       <c r="D463" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E463" s="6">
         <v>45681.155717592592</v>
@@ -11578,7 +11598,7 @@
         <v>13549.09</v>
       </c>
       <c r="D471" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E471" s="6">
         <v>45681.322384259256</v>
@@ -12338,7 +12358,7 @@
         <v>7308.45</v>
       </c>
       <c r="D509" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E509" s="6">
         <v>45588.655717592592</v>
@@ -12518,7 +12538,7 @@
         <v>6685.29</v>
       </c>
       <c r="D518" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E518" s="6">
         <v>45588.822384259256</v>
@@ -12698,7 +12718,7 @@
         <v>1528.07</v>
       </c>
       <c r="D527" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E527" s="6">
         <v>45588.989050925928</v>
@@ -13115,7 +13135,7 @@
         <v>368009</v>
       </c>
       <c r="C548" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D548" s="9" t="s">
         <v>21</v>
@@ -13137,8 +13157,8 @@
       <c r="C549" s="8">
         <v>38.89</v>
       </c>
-      <c r="D549" s="9" t="s">
-        <v>75</v>
+      <c r="D549" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E549" s="6">
         <v>45780.655717592592</v>
@@ -13275,7 +13295,7 @@
         <v>368009</v>
       </c>
       <c r="C556" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D556" s="9" t="s">
         <v>21</v>
@@ -13297,8 +13317,8 @@
       <c r="C557" s="8">
         <v>40.99</v>
       </c>
-      <c r="D557" s="9" t="s">
-        <v>75</v>
+      <c r="D557" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E557" s="6">
         <v>45780.905717592592</v>
@@ -13435,7 +13455,7 @@
         <v>368009</v>
       </c>
       <c r="C564" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D564" s="9" t="s">
         <v>21</v>
@@ -13457,8 +13477,8 @@
       <c r="C565" s="8">
         <v>38.83</v>
       </c>
-      <c r="D565" s="9" t="s">
-        <v>75</v>
+      <c r="D565" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E565" s="6">
         <v>45781.155717592592</v>
@@ -13555,7 +13575,7 @@
         <v>368009</v>
       </c>
       <c r="C570" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D570" s="9" t="s">
         <v>21</v>
@@ -13577,8 +13597,8 @@
       <c r="C571" s="8">
         <v>37.659999999999997</v>
       </c>
-      <c r="D571" s="9" t="s">
-        <v>75</v>
+      <c r="D571" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E571" s="6">
         <v>45781.405717592592</v>
@@ -13635,7 +13655,7 @@
         <v>368009</v>
       </c>
       <c r="C574" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D574" s="9" t="s">
         <v>21</v>
@@ -13657,8 +13677,8 @@
       <c r="C575" s="8">
         <v>37.700000000000003</v>
       </c>
-      <c r="D575" s="9" t="s">
-        <v>75</v>
+      <c r="D575" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E575" s="6">
         <v>45781.655717592592</v>
@@ -13695,7 +13715,7 @@
         <v>368009</v>
       </c>
       <c r="C577" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D577" s="9" t="s">
         <v>21</v>
@@ -14177,8 +14197,8 @@
       <c r="C601" s="9">
         <v>38.03</v>
       </c>
-      <c r="D601" s="14" t="s">
-        <v>75</v>
+      <c r="D601" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E601" s="6">
         <v>45682.655717592592</v>
@@ -14198,7 +14218,7 @@
         <v>4101.4799999999996</v>
       </c>
       <c r="D602" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E602" s="6">
         <v>45682.655717592592</v>
@@ -14255,7 +14275,7 @@
         <v>368009</v>
       </c>
       <c r="C605" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D605" s="14" t="s">
         <v>21</v>
@@ -14317,8 +14337,8 @@
       <c r="C608" s="9">
         <v>41.06</v>
       </c>
-      <c r="D608" s="14" t="s">
-        <v>75</v>
+      <c r="D608" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E608" s="6">
         <v>45682.822384259256</v>
@@ -14338,7 +14358,7 @@
         <v>10963.05</v>
       </c>
       <c r="D609" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E609" s="6">
         <v>45682.822384259256</v>
@@ -14395,7 +14415,7 @@
         <v>368009</v>
       </c>
       <c r="C612" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D612" s="14" t="s">
         <v>21</v>
@@ -14457,8 +14477,8 @@
       <c r="C615" s="9">
         <v>40.26</v>
       </c>
-      <c r="D615" s="14" t="s">
-        <v>75</v>
+      <c r="D615" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E615" s="6">
         <v>45682.989050925928</v>
@@ -14478,7 +14498,7 @@
         <v>12469.04</v>
       </c>
       <c r="D616" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E616" s="6">
         <v>45682.989050925928</v>
@@ -14535,7 +14555,7 @@
         <v>368009</v>
       </c>
       <c r="C619" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D619" s="14" t="s">
         <v>21</v>
@@ -14597,8 +14617,8 @@
       <c r="C622" s="9">
         <v>37.229999999999997</v>
       </c>
-      <c r="D622" s="14" t="s">
-        <v>75</v>
+      <c r="D622" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E622" s="6">
         <v>45683.155717592592</v>
@@ -14618,7 +14638,7 @@
         <v>4316.49</v>
       </c>
       <c r="D623" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E623" s="6">
         <v>45683.155717592592</v>
@@ -14697,8 +14717,8 @@
       <c r="C627" s="9">
         <v>40.26</v>
       </c>
-      <c r="D627" s="14" t="s">
-        <v>75</v>
+      <c r="D627" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E627" s="6">
         <v>45683.322384259256</v>
@@ -14718,7 +14738,7 @@
         <v>10105.709999999999</v>
       </c>
       <c r="D628" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E628" s="6">
         <v>45683.322384259256</v>
@@ -14778,7 +14798,7 @@
         <v>21988.09</v>
       </c>
       <c r="D631" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E631" s="6">
         <v>45683.489050925928</v>
@@ -14837,8 +14857,8 @@
       <c r="C634" s="8">
         <v>37.89</v>
       </c>
-      <c r="D634" s="9" t="s">
-        <v>75</v>
+      <c r="D634" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E634" s="6">
         <v>45562.655717592592</v>
@@ -14977,8 +14997,8 @@
       <c r="C641" s="8">
         <v>51.53</v>
       </c>
-      <c r="D641" s="9" t="s">
-        <v>75</v>
+      <c r="D641" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E641" s="6">
         <v>45562.905717592592</v>
@@ -15117,8 +15137,8 @@
       <c r="C648" s="8">
         <v>36.29</v>
       </c>
-      <c r="D648" s="9" t="s">
-        <v>75</v>
+      <c r="D648" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E648" s="6">
         <v>45563.155717592592</v>
@@ -15237,8 +15257,8 @@
       <c r="C654" s="8">
         <v>40.35</v>
       </c>
-      <c r="D654" s="9" t="s">
-        <v>75</v>
+      <c r="D654" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E654" s="6">
         <v>45563.405717592592</v>
@@ -15317,8 +15337,8 @@
       <c r="C658" s="8">
         <v>38.18</v>
       </c>
-      <c r="D658" s="9" t="s">
-        <v>75</v>
+      <c r="D658" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E658" s="6">
         <v>45563.655717592592</v>
@@ -15377,8 +15397,8 @@
       <c r="C661" s="8">
         <v>25.7</v>
       </c>
-      <c r="D661" s="9" t="s">
-        <v>75</v>
+      <c r="D661" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E661" s="6">
         <v>45563.905717592592</v>
@@ -15418,7 +15438,7 @@
         <v>19539.259999999998</v>
       </c>
       <c r="D663" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E663" s="6">
         <v>45596.655717592592</v>
@@ -15435,7 +15455,7 @@
         <v>368009</v>
       </c>
       <c r="C664" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D664" s="14" t="s">
         <v>21</v>
@@ -15497,8 +15517,8 @@
       <c r="C667" s="9">
         <v>29.42</v>
       </c>
-      <c r="D667" s="14" t="s">
-        <v>75</v>
+      <c r="D667" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E667" s="6">
         <v>45596.655717592592</v>
@@ -15618,7 +15638,7 @@
         <v>1413.89</v>
       </c>
       <c r="D673" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E673" s="6">
         <v>45596.822384259256</v>
@@ -15635,7 +15655,7 @@
         <v>368009</v>
       </c>
       <c r="C674" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D674" s="14" t="s">
         <v>21</v>
@@ -15697,8 +15717,8 @@
       <c r="C677" s="9">
         <v>39.81</v>
       </c>
-      <c r="D677" s="14" t="s">
-        <v>75</v>
+      <c r="D677" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E677" s="6">
         <v>45596.822384259256</v>
@@ -15818,7 +15838,7 @@
         <v>4862.21</v>
       </c>
       <c r="D683" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E683" s="6">
         <v>45596.989050925928</v>
@@ -15835,7 +15855,7 @@
         <v>368009</v>
       </c>
       <c r="C684" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D684" s="14" t="s">
         <v>21</v>
@@ -15897,8 +15917,8 @@
       <c r="C687" s="9">
         <v>40.799999999999997</v>
       </c>
-      <c r="D687" s="14" t="s">
-        <v>75</v>
+      <c r="D687" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E687" s="6">
         <v>45596.989050925928</v>
@@ -15935,7 +15955,7 @@
         <v>23924001</v>
       </c>
       <c r="C689" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D689" s="14" t="s">
         <v>21</v>
@@ -16018,7 +16038,7 @@
         <v>3632.63</v>
       </c>
       <c r="D693" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E693" s="6">
         <v>45597.155717592592</v>
@@ -16035,7 +16055,7 @@
         <v>368009</v>
       </c>
       <c r="C694" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D694" s="14" t="s">
         <v>21</v>
@@ -16097,8 +16117,8 @@
       <c r="C697" s="9">
         <v>41.94</v>
       </c>
-      <c r="D697" s="14" t="s">
-        <v>75</v>
+      <c r="D697" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E697" s="6">
         <v>45597.155717592592</v>
@@ -16297,8 +16317,8 @@
       <c r="C707" s="8">
         <v>39.130000000000003</v>
       </c>
-      <c r="D707" s="9" t="s">
-        <v>75</v>
+      <c r="D707" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E707" s="6">
         <v>45607.655717592592</v>
@@ -16397,8 +16417,8 @@
       <c r="C712" s="8">
         <v>40.28</v>
       </c>
-      <c r="D712" s="9" t="s">
-        <v>75</v>
+      <c r="D712" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E712" s="6">
         <v>45607.905717592592</v>
@@ -16497,8 +16517,8 @@
       <c r="C717" s="8">
         <v>39.71</v>
       </c>
-      <c r="D717" s="9" t="s">
-        <v>75</v>
+      <c r="D717" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E717" s="6">
         <v>45608.155717592592</v>
@@ -16515,7 +16535,7 @@
         <v>23924001</v>
       </c>
       <c r="C718" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D718" s="9" t="s">
         <v>21</v>
@@ -16597,8 +16617,8 @@
       <c r="C722" s="8">
         <v>36.200000000000003</v>
       </c>
-      <c r="D722" s="9" t="s">
-        <v>75</v>
+      <c r="D722" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E722" s="6">
         <v>45608.405717592592</v>
@@ -16657,8 +16677,8 @@
       <c r="C725" s="8">
         <v>39.33</v>
       </c>
-      <c r="D725" s="9" t="s">
-        <v>75</v>
+      <c r="D725" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E725" s="6">
         <v>45608.655717592592</v>
@@ -16758,7 +16778,7 @@
         <v>2479.66</v>
       </c>
       <c r="D730" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E730" s="6">
         <v>45630.655717592592</v>
@@ -16875,7 +16895,7 @@
         <v>368009</v>
       </c>
       <c r="C736" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D736" s="14" t="s">
         <v>21</v>
@@ -16898,7 +16918,7 @@
         <v>14009.86</v>
       </c>
       <c r="D737" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E737" s="6">
         <v>45630.822384259256</v>
@@ -17015,7 +17035,7 @@
         <v>368009</v>
       </c>
       <c r="C743" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D743" s="14" t="s">
         <v>21</v>
@@ -17038,7 +17058,7 @@
         <v>14732.19</v>
       </c>
       <c r="D744" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E744" s="6">
         <v>45630.989050925928</v>
@@ -17155,7 +17175,7 @@
         <v>368009</v>
       </c>
       <c r="C750" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D750" s="14" t="s">
         <v>21</v>
@@ -17178,7 +17198,7 @@
         <v>7368.78</v>
       </c>
       <c r="D751" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E751" s="6">
         <v>45631.155717592592</v>
@@ -17255,7 +17275,7 @@
         <v>368009</v>
       </c>
       <c r="C755" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D755" s="14" t="s">
         <v>21</v>
@@ -17278,7 +17298,7 @@
         <v>11628.72</v>
       </c>
       <c r="D756" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E756" s="6">
         <v>45631.322384259256</v>
@@ -17415,7 +17435,7 @@
         <v>368009</v>
       </c>
       <c r="C763" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D763" s="9" t="s">
         <v>21</v>
@@ -17515,7 +17535,7 @@
         <v>368009</v>
       </c>
       <c r="C768" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D768" s="9" t="s">
         <v>21</v>
@@ -17615,7 +17635,7 @@
         <v>368009</v>
       </c>
       <c r="C773" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D773" s="9" t="s">
         <v>21</v>
@@ -17818,7 +17838,7 @@
         <v>0</v>
       </c>
       <c r="D783" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E783" s="6">
         <v>45683.655717592592</v>
@@ -17935,7 +17955,7 @@
         <v>368009</v>
       </c>
       <c r="C789" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D789" s="14" t="s">
         <v>21</v>
@@ -17978,7 +17998,7 @@
         <v>12245.7</v>
       </c>
       <c r="D791" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E791" s="6">
         <v>45683.822384259256</v>
@@ -18095,7 +18115,7 @@
         <v>368009</v>
       </c>
       <c r="C797" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D797" s="14" t="s">
         <v>21</v>
@@ -18138,7 +18158,7 @@
         <v>7373.16</v>
       </c>
       <c r="D799" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E799" s="6">
         <v>45683.989050925928</v>
@@ -18255,7 +18275,7 @@
         <v>368009</v>
       </c>
       <c r="C805" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D805" s="14" t="s">
         <v>21</v>
@@ -18298,7 +18318,7 @@
         <v>5516.06</v>
       </c>
       <c r="D807" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E807" s="6">
         <v>45684.155717592592</v>
@@ -18395,7 +18415,7 @@
         <v>368009</v>
       </c>
       <c r="C812" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D812" s="14" t="s">
         <v>21</v>
@@ -18438,7 +18458,7 @@
         <v>0</v>
       </c>
       <c r="D814" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E814" s="6">
         <v>45684.322384259256</v>
@@ -18515,7 +18535,7 @@
         <v>368009</v>
       </c>
       <c r="C818" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D818" s="14" t="s">
         <v>21</v>
@@ -19115,7 +19135,7 @@
         <v>368009</v>
       </c>
       <c r="C848" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D848" s="14" t="s">
         <v>21</v>
@@ -19295,7 +19315,7 @@
         <v>368009</v>
       </c>
       <c r="C857" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D857" s="14" t="s">
         <v>21</v>
@@ -19455,7 +19475,7 @@
         <v>23924001</v>
       </c>
       <c r="C865" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D865" s="14" t="s">
         <v>21</v>
@@ -19475,7 +19495,7 @@
         <v>368009</v>
       </c>
       <c r="C866" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D866" s="14" t="s">
         <v>21</v>
@@ -19595,7 +19615,7 @@
         <v>23924001</v>
       </c>
       <c r="C872" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D872" s="14" t="s">
         <v>21</v>
@@ -19615,7 +19635,7 @@
         <v>368009</v>
       </c>
       <c r="C873" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D873" s="14" t="s">
         <v>21</v>
@@ -19695,7 +19715,7 @@
         <v>368009</v>
       </c>
       <c r="C877" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D877" s="14" t="s">
         <v>21</v>
@@ -19735,7 +19755,7 @@
         <v>368009</v>
       </c>
       <c r="C879" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D879" s="14" t="s">
         <v>21</v>
@@ -19895,7 +19915,7 @@
         <v>368009</v>
       </c>
       <c r="C887" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D887" s="14" t="s">
         <v>21</v>
@@ -20035,7 +20055,7 @@
         <v>368009</v>
       </c>
       <c r="C894" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D894" s="14" t="s">
         <v>21</v>
@@ -20175,7 +20195,7 @@
         <v>368009</v>
       </c>
       <c r="C901" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D901" s="14" t="s">
         <v>21</v>
@@ -20295,7 +20315,7 @@
         <v>368009</v>
       </c>
       <c r="C907" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D907" s="14" t="s">
         <v>21</v>
@@ -20415,7 +20435,7 @@
         <v>368009</v>
       </c>
       <c r="C913" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D913" s="14" t="s">
         <v>21</v>
@@ -20555,7 +20575,7 @@
         <v>368009</v>
       </c>
       <c r="C920" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D920" s="9" t="s">
         <v>21</v>
@@ -20675,7 +20695,7 @@
         <v>368009</v>
       </c>
       <c r="C926" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D926" s="9" t="s">
         <v>21</v>
@@ -20795,7 +20815,7 @@
         <v>368009</v>
       </c>
       <c r="C932" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D932" s="9" t="s">
         <v>21</v>
@@ -20915,7 +20935,7 @@
         <v>368009</v>
       </c>
       <c r="C938" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D938" s="9" t="s">
         <v>21</v>
@@ -21035,7 +21055,7 @@
         <v>368009</v>
       </c>
       <c r="C944" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D944" s="9" t="s">
         <v>21</v>
@@ -21115,7 +21135,7 @@
         <v>368009</v>
       </c>
       <c r="C948" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D948" s="9" t="s">
         <v>21</v>
@@ -21218,7 +21238,7 @@
         <v>3802.02</v>
       </c>
       <c r="D953" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E953" s="6">
         <v>45630.655717592592</v>
@@ -21255,7 +21275,7 @@
         <v>368009</v>
       </c>
       <c r="C955" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D955" s="9" t="s">
         <v>21</v>
@@ -21275,7 +21295,7 @@
         <v>23924001</v>
       </c>
       <c r="C956" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D956" s="9" t="s">
         <v>21</v>
@@ -21378,7 +21398,7 @@
         <v>13340.77</v>
       </c>
       <c r="D961" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E961" s="6">
         <v>45630.905717592592</v>
@@ -21415,7 +21435,7 @@
         <v>368009</v>
       </c>
       <c r="C963" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D963" s="9" t="s">
         <v>21</v>
@@ -21538,7 +21558,7 @@
         <v>769.26</v>
       </c>
       <c r="D969" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E969" s="6">
         <v>45631.155717592592</v>
@@ -21575,7 +21595,7 @@
         <v>368009</v>
       </c>
       <c r="C971" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D971" s="9" t="s">
         <v>21</v>
@@ -21658,7 +21678,7 @@
         <v>4624.46</v>
       </c>
       <c r="D975" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E975" s="6">
         <v>45631.405717592592</v>
@@ -21695,7 +21715,7 @@
         <v>368009</v>
       </c>
       <c r="C977" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D977" s="9" t="s">
         <v>21</v>
@@ -21778,7 +21798,7 @@
         <v>227.91</v>
       </c>
       <c r="D981" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E981" s="6">
         <v>45631.655717592592</v>
@@ -21858,7 +21878,7 @@
         <v>3698</v>
       </c>
       <c r="D985" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E985" s="6">
         <v>45631.905717592592</v>
@@ -21917,8 +21937,8 @@
       <c r="C988" s="9">
         <v>61.85</v>
       </c>
-      <c r="D988" s="14" t="s">
-        <v>75</v>
+      <c r="D988" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E988" s="6">
         <v>45734.655717592592</v>
@@ -21935,7 +21955,7 @@
         <v>368009</v>
       </c>
       <c r="C989" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D989" s="14" t="s">
         <v>21</v>
@@ -21998,7 +22018,7 @@
         <v>1433.23</v>
       </c>
       <c r="D992" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E992" s="6">
         <v>45734.655717592592</v>
@@ -22057,8 +22077,8 @@
       <c r="C995" s="9">
         <v>41.13</v>
       </c>
-      <c r="D995" s="14" t="s">
-        <v>75</v>
+      <c r="D995" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E995" s="6">
         <v>45734.822384259256</v>
@@ -22075,7 +22095,7 @@
         <v>368009</v>
       </c>
       <c r="C996" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D996" s="14" t="s">
         <v>21</v>
@@ -22138,7 +22158,7 @@
         <v>13869.55</v>
       </c>
       <c r="D999" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E999" s="6">
         <v>45734.822384259256</v>
@@ -22197,8 +22217,8 @@
       <c r="C1002" s="9">
         <v>38.6</v>
       </c>
-      <c r="D1002" s="14" t="s">
-        <v>75</v>
+      <c r="D1002" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1002" s="6">
         <v>45734.989050925928</v>
@@ -22215,7 +22235,7 @@
         <v>368009</v>
       </c>
       <c r="C1003" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1003" s="14" t="s">
         <v>21</v>
@@ -22278,7 +22298,7 @@
         <v>2537.16</v>
       </c>
       <c r="D1006" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1006" s="6">
         <v>45734.989050925928</v>
@@ -22317,8 +22337,8 @@
       <c r="C1008" s="9">
         <v>39.1</v>
       </c>
-      <c r="D1008" s="14" t="s">
-        <v>75</v>
+      <c r="D1008" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1008" s="6">
         <v>45735.155717592592</v>
@@ -23477,8 +23497,8 @@
       <c r="C1066" s="9">
         <v>39.11</v>
       </c>
-      <c r="D1066" s="14" t="s">
-        <v>75</v>
+      <c r="D1066" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1066" s="6">
         <v>45796.655717592592</v>
@@ -23558,7 +23578,7 @@
         <v>6357.68</v>
       </c>
       <c r="D1070" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1070" s="6">
         <v>45796.655717592592</v>
@@ -23617,8 +23637,8 @@
       <c r="C1073" s="9">
         <v>38.72</v>
       </c>
-      <c r="D1073" s="14" t="s">
-        <v>75</v>
+      <c r="D1073" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1073" s="6">
         <v>45796.822384259256</v>
@@ -23698,7 +23718,7 @@
         <v>1156.54</v>
       </c>
       <c r="D1077" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1077" s="6">
         <v>45796.822384259256</v>
@@ -23757,8 +23777,8 @@
       <c r="C1080" s="9">
         <v>37.74</v>
       </c>
-      <c r="D1080" s="14" t="s">
-        <v>75</v>
+      <c r="D1080" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1080" s="6">
         <v>45796.989050925928</v>
@@ -23838,7 +23858,7 @@
         <v>12451.47</v>
       </c>
       <c r="D1084" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1084" s="6">
         <v>45796.989050925928</v>
@@ -23958,7 +23978,7 @@
         <v>13142.67</v>
       </c>
       <c r="D1090" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1090" s="6">
         <v>45797.155717592592</v>
@@ -24097,8 +24117,8 @@
       <c r="C1097" s="8">
         <v>39.82</v>
       </c>
-      <c r="D1097" s="9" t="s">
-        <v>75</v>
+      <c r="D1097" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1097" s="6">
         <v>45587.655717592592</v>
@@ -24118,7 +24138,7 @@
         <v>21543.82</v>
       </c>
       <c r="D1098" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1098" s="6">
         <v>45587.655717592592</v>
@@ -24155,7 +24175,7 @@
         <v>368009</v>
       </c>
       <c r="C1100" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1100" s="9" t="s">
         <v>21</v>
@@ -24175,7 +24195,7 @@
         <v>23924001</v>
       </c>
       <c r="C1101" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1101" s="9" t="s">
         <v>21</v>
@@ -24217,8 +24237,8 @@
       <c r="C1103" s="8">
         <v>41.97</v>
       </c>
-      <c r="D1103" s="9" t="s">
-        <v>75</v>
+      <c r="D1103" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1103" s="6">
         <v>45587.905717592592</v>
@@ -24238,7 +24258,7 @@
         <v>10610.85</v>
       </c>
       <c r="D1104" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1104" s="6">
         <v>45587.905717592592</v>
@@ -24275,7 +24295,7 @@
         <v>368009</v>
       </c>
       <c r="C1106" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1106" s="9" t="s">
         <v>21</v>
@@ -24337,8 +24357,8 @@
       <c r="C1109" s="8">
         <v>36.409999999999997</v>
       </c>
-      <c r="D1109" s="9" t="s">
-        <v>75</v>
+      <c r="D1109" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1109" s="6">
         <v>45588.155717592592</v>
@@ -24358,7 +24378,7 @@
         <v>5985.49</v>
       </c>
       <c r="D1110" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1110" s="6">
         <v>45588.155717592592</v>
@@ -24395,7 +24415,7 @@
         <v>368009</v>
       </c>
       <c r="C1112" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1112" s="9" t="s">
         <v>21</v>
@@ -24437,8 +24457,8 @@
       <c r="C1114" s="8">
         <v>32.39</v>
       </c>
-      <c r="D1114" s="9" t="s">
-        <v>75</v>
+      <c r="D1114" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1114" s="6">
         <v>45588.405717592592</v>
@@ -24458,7 +24478,7 @@
         <v>14592.5</v>
       </c>
       <c r="D1115" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1115" s="6">
         <v>45588.405717592592</v>
@@ -24498,7 +24518,7 @@
         <v>3011.89</v>
       </c>
       <c r="D1117" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1117" s="6">
         <v>45588.655717592592</v>
@@ -24518,7 +24538,7 @@
         <v>4152.3</v>
       </c>
       <c r="D1118" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1118" s="6">
         <v>45588.905717592592</v>
@@ -24555,7 +24575,7 @@
         <v>368009</v>
       </c>
       <c r="C1120" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1120" s="14" t="s">
         <v>21</v>
@@ -24618,7 +24638,7 @@
         <v>10636.96</v>
       </c>
       <c r="D1123" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1123" s="6">
         <v>45606.655717592592</v>
@@ -24657,8 +24677,8 @@
       <c r="C1125" s="9">
         <v>36.659999999999997</v>
       </c>
-      <c r="D1125" s="14" t="s">
-        <v>75</v>
+      <c r="D1125" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1125" s="6">
         <v>45606.655717592592</v>
@@ -24715,7 +24735,7 @@
         <v>368009</v>
       </c>
       <c r="C1128" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1128" s="14" t="s">
         <v>21</v>
@@ -24778,7 +24798,7 @@
         <v>728.21</v>
       </c>
       <c r="D1131" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1131" s="6">
         <v>45606.822384259256</v>
@@ -24817,8 +24837,8 @@
       <c r="C1133" s="9">
         <v>40.6</v>
       </c>
-      <c r="D1133" s="14" t="s">
-        <v>75</v>
+      <c r="D1133" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1133" s="6">
         <v>45606.822384259256</v>
@@ -24875,7 +24895,7 @@
         <v>368009</v>
       </c>
       <c r="C1136" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1136" s="14" t="s">
         <v>21</v>
@@ -24938,7 +24958,7 @@
         <v>8442.0300000000007</v>
       </c>
       <c r="D1139" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1139" s="6">
         <v>45606.989050925928</v>
@@ -24977,8 +24997,8 @@
       <c r="C1141" s="9">
         <v>41.37</v>
       </c>
-      <c r="D1141" s="14" t="s">
-        <v>75</v>
+      <c r="D1141" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E1141" s="6">
         <v>45606.989050925928</v>
@@ -25035,7 +25055,7 @@
         <v>368009</v>
       </c>
       <c r="C1144" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1144" s="14" t="s">
         <v>21</v>
@@ -25098,7 +25118,7 @@
         <v>11940.63</v>
       </c>
       <c r="D1147" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1147" s="6">
         <v>45607.155717592592</v>
@@ -25155,7 +25175,7 @@
         <v>368009</v>
       </c>
       <c r="C1150" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1150" s="14" t="s">
         <v>21</v>
@@ -25255,7 +25275,7 @@
         <v>368009</v>
       </c>
       <c r="C1155" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1155" s="14" t="s">
         <v>21</v>
@@ -25325,6 +25345,1326 @@
       </c>
       <c r="F1158" s="6">
         <v>45607.573078703703</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1159" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1159" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1159" s="9">
+        <v>7</v>
+      </c>
+      <c r="D1159" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1159" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1159" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1160" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1160" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1160" s="9">
+        <v>3500</v>
+      </c>
+      <c r="D1160" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1160" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1160" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1161" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1161" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1161" s="9">
+        <v>38</v>
+      </c>
+      <c r="D1161" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1161" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1161" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1162" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1162" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1162" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1162" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1162" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1162" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1163" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1163" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1163" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1163" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1163" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1163" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1164" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1164" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1164" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1164" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1164" s="6">
+        <v>45658.375</v>
+      </c>
+      <c r="F1164" s="6">
+        <v>45658.416666666657</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1165" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1165" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1165" s="9">
+        <v>14</v>
+      </c>
+      <c r="D1165" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1165" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1165" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1166" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1166" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1166" s="9">
+        <v>3500</v>
+      </c>
+      <c r="D1166" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1166" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1166" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1167" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1167" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1167" s="9">
+        <v>39</v>
+      </c>
+      <c r="D1167" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1167" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1167" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1168" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1168" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1168" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1168" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1168" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1168" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1169" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1169" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1169" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1169" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1169" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1169" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1170" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1170" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1170" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1170" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1170" s="6">
+        <v>45659.375</v>
+      </c>
+      <c r="F1170" s="6">
+        <v>45659.416666666657</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1171" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1171" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1171" s="9">
+        <v>17</v>
+      </c>
+      <c r="D1171" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1171" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1171" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1172" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1172" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1172" s="9">
+        <v>3500</v>
+      </c>
+      <c r="D1172" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1172" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1172" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1173" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1173" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1173" s="9">
+        <v>40.1</v>
+      </c>
+      <c r="D1173" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1173" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1173" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1174" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1174" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1174" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1174" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1174" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1174" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1175" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1175" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1175" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1175" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1175" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1175" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1176" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1176" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1176" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1176" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1176" s="6">
+        <v>45660.375</v>
+      </c>
+      <c r="F1176" s="6">
+        <v>45660.416666666657</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1177" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1177" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1177" s="9">
+        <v>10</v>
+      </c>
+      <c r="D1177" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1177" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1177" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1178" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1178" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1178" s="9">
+        <v>7000</v>
+      </c>
+      <c r="D1178" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1178" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1178" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1179" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1179" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1179" s="9">
+        <v>40</v>
+      </c>
+      <c r="D1179" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1179" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1179" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1180" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1180" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1180" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1180" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1180" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1180" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1181" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1181" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1181" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1181" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1181" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1181" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1182" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1182" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1182" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1182" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1182" s="6">
+        <v>45661.375</v>
+      </c>
+      <c r="F1182" s="6">
+        <v>45661.416666666657</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1183" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1183" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1183" s="9">
+        <v>14</v>
+      </c>
+      <c r="D1183" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1183" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1183" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1184" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1184" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1184" s="9">
+        <v>7000</v>
+      </c>
+      <c r="D1184" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1184" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1184" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1185" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1185" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1185" s="9">
+        <v>38.4</v>
+      </c>
+      <c r="D1185" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1185" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1185" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1186" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1186" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1186" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1186" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1186" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1186" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1187" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1187" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1187" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1187" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1187" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1187" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1188" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1188" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1188" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1188" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1188" s="6">
+        <v>45662.375</v>
+      </c>
+      <c r="F1188" s="6">
+        <v>45662.416666666657</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1189" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1189" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1189" s="9">
+        <v>17</v>
+      </c>
+      <c r="D1189" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1189" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1189" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1190" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1190" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1190" s="9">
+        <v>7000</v>
+      </c>
+      <c r="D1190" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1190" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1190" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1191" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1191" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1191" s="9">
+        <v>39.5</v>
+      </c>
+      <c r="D1191" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1191" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1191" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1192" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1192" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1192" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1192" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1192" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1192" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1193" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1193" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1193" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1193" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1193" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1193" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1194" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1194" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1194" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1194" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1194" s="6">
+        <v>45663.375</v>
+      </c>
+      <c r="F1194" s="6">
+        <v>45663.416666666657</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1195" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1195" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1195" s="9">
+        <v>11</v>
+      </c>
+      <c r="D1195" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1195" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1195" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1196" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1196" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1196" s="9">
+        <v>12000</v>
+      </c>
+      <c r="D1196" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1196" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1196" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1197" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1197" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1197" s="9">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="D1197" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1197" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1197" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1198" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1198" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1198" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1198" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1198" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1198" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1199" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1199" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1199" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1199" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1199" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1199" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1200" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1200" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1200" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1200" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1200" s="6">
+        <v>45664.375</v>
+      </c>
+      <c r="F1200" s="6">
+        <v>45664.416666666657</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1201" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1201" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1201" s="9">
+        <v>14</v>
+      </c>
+      <c r="D1201" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1201" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1201" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1202" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1202" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1202" s="9">
+        <v>12000</v>
+      </c>
+      <c r="D1202" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1202" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1202" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1203" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1203" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1203" s="9">
+        <v>40</v>
+      </c>
+      <c r="D1203" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1203" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1203" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1204" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1204" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1204" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1204" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1204" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1204" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1205" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1205" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1205" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1205" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1205" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1205" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1206" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1206" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1206" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1206" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1206" s="6">
+        <v>45665.375</v>
+      </c>
+      <c r="F1206" s="6">
+        <v>45665.416666666657</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1207" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1207" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1207" s="9">
+        <v>17</v>
+      </c>
+      <c r="D1207" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1207" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1207" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1208" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1208" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1208" s="9">
+        <v>12000</v>
+      </c>
+      <c r="D1208" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1208" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1208" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1209" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1209" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1209" s="9">
+        <v>38.6</v>
+      </c>
+      <c r="D1209" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1209" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1209" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1210" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1210" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1210" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1210" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1210" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1210" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1211" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1211" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1211" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1211" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1211" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1211" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1212" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1212" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1212" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1212" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1212" s="6">
+        <v>45666.375</v>
+      </c>
+      <c r="F1212" s="6">
+        <v>45666.416666666657</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1213" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1213" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1213" s="9">
+        <v>10</v>
+      </c>
+      <c r="D1213" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1213" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1213" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1214" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1214" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1214" s="9">
+        <v>7000</v>
+      </c>
+      <c r="D1214" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1214" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1214" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1215" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1215" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1215" s="9">
+        <v>39</v>
+      </c>
+      <c r="D1215" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1215" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1215" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1216" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1216" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1216" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1216" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1216" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1216" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1217" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1217" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1217" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1217" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1217" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1217" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1218" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1218" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1218" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1218" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1218" s="6">
+        <v>45667.416666666664</v>
+      </c>
+      <c r="F1218" s="6">
+        <v>45667.416666666664</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1219" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1219" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1219" s="9">
+        <v>17</v>
+      </c>
+      <c r="D1219" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1219" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1219" s="6">
+        <v>45668.416666666664</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1220" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1220" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1220" s="9">
+        <v>12000</v>
+      </c>
+      <c r="D1220" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1220" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1220" s="6">
+        <v>45668.416666666664</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1221" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1221" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1221" s="9">
+        <v>40</v>
+      </c>
+      <c r="D1221" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1221" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1221" s="6">
+        <v>45668.416666666664</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1222" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1222" s="5">
+        <v>43724002</v>
+      </c>
+      <c r="C1222" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1222" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1222" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1222" s="6">
+        <v>45668.416666666664</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1223" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1223" s="5">
+        <v>368009</v>
+      </c>
+      <c r="C1223" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1223" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1223" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1223" s="6">
+        <v>45668.416666666664</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1224" s="5">
+        <v>147258369</v>
+      </c>
+      <c r="B1224" s="5">
+        <v>23924001</v>
+      </c>
+      <c r="C1224" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1224" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1224" s="6">
+        <v>45668.416666666664</v>
+      </c>
+      <c r="F1224" s="6">
+        <v>45668.416666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments + __main__ update
</commit_message>
<xml_diff>
--- a/data/project_db.xlsx
+++ b/data/project_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\cdss-dev-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruson\OneDrive\מסמכים\תואר שני\גרסה סופית פרויקט של ארז\CDSS-Dev-Project-main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B499A8F8-E688-4D0C-A6DD-7DCAEA695BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0DC91F-BF7A-4544-9C21-D14EE283EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-2325" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="84">
   <si>
     <t>Value</t>
   </si>
@@ -336,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -344,11 +344,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -397,6 +412,12 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1395,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1273"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A1215" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1245" sqref="A1245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -26918,8 +26939,8 @@
       <c r="A1250" s="3">
         <v>567890126</v>
       </c>
-      <c r="B1250" s="3">
-        <v>23924001</v>
+      <c r="B1250" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="C1250" s="6">
         <v>17</v>
@@ -26938,8 +26959,8 @@
       <c r="A1251" s="3">
         <v>678901237</v>
       </c>
-      <c r="B1251" s="3" t="s">
-        <v>35</v>
+      <c r="B1251" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="C1251" s="6">
         <v>12000</v>

</xml_diff>